<commit_message>
adicionando seleção via mapa e filtros multiplos
</commit_message>
<xml_diff>
--- a/app/static/media/xlsx/temp.xlsx
+++ b/app/static/media/xlsx/temp.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,71 +541,76 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MSP21</t>
+          <t>MGO12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Av. Maracanã, 882 -Frente ao Shopping Tijuca </t>
+          <t xml:space="preserve">Av Denise Cristina Da Rocha, Em Frente Braunas </t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-22.9227479</v>
+        <v>-19.802656</v>
       </c>
       <c r="D2" t="n">
-        <v>-43.235922</v>
+        <v>-44.0040275</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://i.ibb.co/5LsGKKN/Av-Maracan-882-Frente-ao-Shopping-Tijuca-Sent-Barra.png</t>
+          <t>https://i.ibb.co/q5xpNnh/AV-DENISE-CRISTINA-DA-ROCHA-EM-FRENTE-BRAUNAS-19-48-09-7-S-44-00-14-5-W.jpg</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rio de Janeiro </t>
+          <t>Ribeirão das Neves</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Minas Gerais</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>brasil</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Empena PREMIUM   7x12</t>
+          <t xml:space="preserve">Outdoor </t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MFD457</t>
+          <t>MRC10</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Alameda Oscar Niemeyer 1280 – Em Frente Ao Cone’xao Aeroporto – Vila Da Serra  </t>
+          <t>Av.Brasilia proximo ao clube Lago Azul Duquesa II.</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-19.9754177</v>
+        <v>-19.7768379</v>
       </c>
       <c r="D3" t="n">
-        <v>-43.9386911</v>
+        <v>-43.8970794</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://i.ibb.co/ctgh5YD/ALAMEDA-OSCAR-NIEMEYER-1280-NOVA-LIMA.jpg</t>
+          <t>https://i.ibb.co/KmtBT8P/Av-Brasilia-proximo-ao-clube-Lago-Azul-Duquesa-II.jpg</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Vila Da Serra</t>
+          <t>Bonó</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Nova Lima</t>
+          <t>Santa Luzia</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -615,108 +620,12 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>brasil</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Banca LED</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>MEM33</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Alameda Da Serra, 418, Frente Ao Biocor</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>-19.9812221</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-43.9442775</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>http://uploaddeimagens.com.br/imagens/ledb_001_alamedadaserra418-jpg-0c9ec6a0-7e3d-485a-b5f8-8bc8c8a1eea0</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Belvedere</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Nova Lima</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Minas Gerais</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>brasil</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Banca LED</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>MEM34</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Alameda Da Serra, 858, Frente Ao Rest. Djalma</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>-19.9777656</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-43.94146972</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>http://uploaddeimagens.com.br/imagens/ledb_002_alamedadaserra858-jpg-6cdbcb64-3668-4417-89c7-f405e1c1ad1e</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Belvedere</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Nova Lima</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Minas Gerais</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>brasil</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Banca LED</t>
+          <t xml:space="preserve">Outdoor </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
acrescentando ordenar por e mudando a busca por id para decrescente
</commit_message>
<xml_diff>
--- a/app/static/media/xlsx/temp.xlsx
+++ b/app/static/media/xlsx/temp.xlsx
@@ -429,17 +429,17 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Endereço</t>
+          <t>Dirección</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Latidude</t>
+          <t>Latitud</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Longitude</t>
+          <t>Longitud</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -449,17 +449,17 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Bairro</t>
+          <t>Barrio</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Referência</t>
+          <t>Referencia</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Cidade</t>
+          <t>Ciudad</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
@@ -469,7 +469,7 @@
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Estado</t>
+          <t>Provincia</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
@@ -494,7 +494,7 @@
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>Valor tabela</t>
+          <t>Valor de la tabla</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
@@ -504,12 +504,12 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>Produção</t>
+          <t>Producción</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>Observações</t>
+          <t>Comentarios</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
@@ -524,7 +524,7 @@
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>Custo líquido</t>
+          <t>Costo neto</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
@@ -534,88 +534,68 @@
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>Comentários internos</t>
+          <t>Comentarios internos</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MGO12</t>
+          <t>MDV40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Av Denise Cristina Da Rocha, Em Frente Braunas </t>
+          <t>Av. Torquato Tapajós,  3741, Prox VIDEOLAR e AMBEV - Novo Israel - Sent Centro</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-19.802656</v>
+        <v>-3.0251296</v>
       </c>
       <c r="D2" t="n">
-        <v>-44.0040275</v>
+        <v>-60.0214348</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://i.ibb.co/q5xpNnh/AV-DENISE-CRISTINA-DA-ROCHA-EM-FRENTE-BRAUNAS-19-48-09-7-S-44-00-14-5-W.jpg</t>
+          <t>https://i.ibb.co/Xk6bLnt/Av-Torquato-Tapaj-s-3741-Prox-VIDEOLAR-e-AMBEV-Novo-Israel.jpg</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Ribeirão das Neves</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Minas Gerais</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Brasil</t>
+          <t>Manaus</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Outdoor </t>
+          <t>10x4</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MRC10</t>
+          <t>MMK10</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Av.Brasilia proximo ao clube Lago Azul Duquesa II.</t>
+          <t>AV. PERIMETRAL, (APAE)  - SENTIDO BOLDA DO ELDORADO - próximo do Shopping Manauara e em frente ao CSU</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-19.7768379</v>
+        <v>-3.0857</v>
       </c>
       <c r="D3" t="n">
-        <v>-43.8970794</v>
+        <v>-60.01127</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://i.ibb.co/KmtBT8P/Av-Brasilia-proximo-ao-clube-Lago-Azul-Duquesa-II.jpg</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Bonó</t>
+          <t>https://i.ibb.co/bRrJQVp/AV-PERIMETRAL-APAE-SENTIDO-BOLDA-DO-ELDORADO.png</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Santa Luzia</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Minas Gerais</t>
+          <t>Manaus</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -625,7 +605,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Outdoor </t>
+          <t>10x4</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
criando checkbox de marcadores incompleto
</commit_message>
<xml_diff>
--- a/app/static/media/xlsx/temp.xlsx
+++ b/app/static/media/xlsx/temp.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,61 +541,91 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MDV40</t>
+          <t>MSAT36</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Av. Torquato Tapajós,  3741, Prox VIDEOLAR e AMBEV - Novo Israel - Sent Centro</t>
+          <t>Av. Rivadavia 7589</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-3.0251296</v>
+        <v>-34.6314059</v>
       </c>
       <c r="D2" t="n">
-        <v>-60.0214348</v>
+        <v>-58.4720002</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://i.ibb.co/Xk6bLnt/Av-Torquato-Tapaj-s-3741-Prox-VIDEOLAR-e-AMBEV-Novo-Israel.jpg</t>
+          <t>https://i.ibb.co/fr7R0FD/Av-Rivadavia-7589-cara-hacia-Gral-Paz.jpg</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Flores</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Manaus</t>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>10x4</t>
+          <t>Medianera</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Atacama</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MMK10</t>
+          <t>MSAT42</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AV. PERIMETRAL, (APAE)  - SENTIDO BOLDA DO ELDORADO - próximo do Shopping Manauara e em frente ao CSU</t>
+          <t>Av.Gaona 1770</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-3.0857</v>
+        <v>-34.6110181</v>
       </c>
       <c r="D3" t="n">
-        <v>-60.01127</v>
+        <v>-58.4530194</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://i.ibb.co/bRrJQVp/AV-PERIMETRAL-APAE-SENTIDO-BOLDA-DO-ELDORADO.png</t>
+          <t>https://i.ibb.co/xFfKQp6/Av-Gaona-1770.jpg</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Caballito</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Manaus</t>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>CABA</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -605,7 +635,156 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>10x4</t>
+          <t>Medianera</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Atacama</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MSAT43</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Av.Juan B.Justo 8324</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>-34.6341896</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-58.5057639</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co/cJTHyc7/Av-Juan-B-Justo-8324.jpg</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Villa Luro</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Medianera</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Atacama</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MSAT46</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Av. San Martín 7035 (tránsito a Provincia)</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>-34.5911444</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-58.5125877</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co/dMzv67d/Av-San-Mart-n-7035-hacia-Provincia.jpg</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Devoto</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Medianera</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Atacama</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>MA63</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>AV.TRIUNVIRATO 3700</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>-34.6117381</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-58.4233365</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co/K6kDR7S/Rua-Jo-o-C-mara-pr-ximo-a-Av-das-Flores-Trajeto-para-Zona-Norte.jpg</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pantalla </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
selecionar marcadores por formato funcionando em Lista
</commit_message>
<xml_diff>
--- a/app/static/media/xlsx/temp.xlsx
+++ b/app/static/media/xlsx/temp.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,38 +541,38 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MSAT36</t>
+          <t>MSAT30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Av. Rivadavia 7589</t>
+          <t>Au.Panamericana _Blas Parera 1297|</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-34.6314059</v>
+        <v>-34.5354354</v>
       </c>
       <c r="D2" t="n">
-        <v>-58.4720002</v>
+        <v>-58.5021847</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://i.ibb.co/fr7R0FD/Av-Rivadavia-7589-cara-hacia-Gral-Paz.jpg</t>
+          <t>https://i.ibb.co/x215Lvb/Blas-Parera-1267-Au-Panamericana.jpg</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Flores</t>
+          <t>Vicente Lopez</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>CABA</t>
+          <t>BUENOS AIRES</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>CABA</t>
+          <t>GBA NORTE</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -582,7 +582,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Medianera</t>
+          <t>Cartel Espectacular Doble Faz</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -594,38 +594,38 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MSAT42</t>
+          <t>MSAT33</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Av.Gaona 1770</t>
+          <t>Av. Crisólogo Larralde 899</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-34.6110181</v>
+        <v>-34.6766898</v>
       </c>
       <c r="D3" t="n">
-        <v>-58.4530194</v>
+        <v>-58.4598458</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://i.ibb.co/xFfKQp6/Av-Gaona-1770.jpg</t>
+          <t>https://i.ibb.co/q0v38Mj/Av-Cris-logo-Larralde-899-Avellaneda-GBA.jpg</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Caballito</t>
+          <t>Avellaneda</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>CABA</t>
+          <t>BUENOS AIRES</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>CABA</t>
+          <t>GBA SUR</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Medianera</t>
+          <t>Cartel Espectacular Simple Faz</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -647,38 +647,38 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MSAT43</t>
+          <t>MSAT34</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Av.Juan B.Justo 8324</t>
+          <t>Av. Del Libertador 240</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-34.6341896</v>
+        <v>-34.532315</v>
       </c>
       <c r="D4" t="n">
-        <v>-58.5057639</v>
+        <v>-58.4712099</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://i.ibb.co/cJTHyc7/Av-Juan-B-Justo-8324.jpg</t>
+          <t>https://i.ibb.co/VCHZWdj/Av-Del-Libertador-240-Vte-L-pez.jpg</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Villa Luro</t>
+          <t>Vicente Lopez</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>CABA</t>
+          <t>BUENOS AIRES</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>CABA</t>
+          <t>GBA NORTE</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -694,97 +694,6 @@
       <c r="S4" t="inlineStr">
         <is>
           <t>Atacama</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>MSAT46</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Av. San Martín 7035 (tránsito a Provincia)</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>-34.5911444</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-58.5125877</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>https://i.ibb.co/dMzv67d/Av-San-Mart-n-7035-hacia-Provincia.jpg</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Devoto</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>CABA</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>CABA</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Medianera</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>Atacama</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>MA63</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>AV.TRIUNVIRATO 3700</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>-34.6117381</v>
-      </c>
-      <c r="D6" t="n">
-        <v>-58.4233365</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>https://i.ibb.co/K6kDR7S/Rua-Jo-o-C-mara-pr-ximo-a-Av-das-Flores-Trajeto-para-Zona-Norte.jpg</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>CABA</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Pantalla </t>
         </is>
       </c>
     </row>

</xml_diff>